<commit_message>
able to slice and combine images now for object detection
</commit_message>
<xml_diff>
--- a/LED Images Data/Data.xlsx
+++ b/LED Images Data/Data.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="36">
   <si>
     <t>Training Set 1</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Object Detection</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>1.35 seconds</t>
+  </si>
+  <si>
+    <t>Detection Time (per well)</t>
   </si>
 </sst>
 </file>
@@ -173,9 +182,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,16 +488,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
     <col min="3" max="18" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -674,7 +685,7 @@
       <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -728,7 +739,7 @@
       <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -833,8 +844,10 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="1">
+        <v>200</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -859,8 +872,10 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -885,8 +900,10 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="1">
+        <v>0.82099999999999995</v>
+      </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -913,8 +930,10 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -923,6 +942,36 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="21" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T21">
+        <f>+I12</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>